<commit_message>
Mix brand and mix model panels modified
</commit_message>
<xml_diff>
--- a/public/bulk -product-sheet-sample.xlsx
+++ b/public/bulk -product-sheet-sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26717"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27207"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4706C8BA-A675-4F84-9A88-E7B00B3DE244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F24EC784-626B-4C90-A57B-2CD1B51547BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,6 +14,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Vendor-SKU-ID</t>
   </si>
@@ -48,13 +51,16 @@
   </si>
   <si>
     <t>Jack-Type</t>
+  </si>
+  <si>
+    <t>Variant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +73,14 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,12 +109,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -416,9 +432,10 @@
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,6 +454,12 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15">
+      <c r="E4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>